<commit_message>
commit Class diagram, Querys/CREATE_TABLES.sql
</commit_message>
<xml_diff>
--- a/Documents/DB_Tables_20141229.xlsx
+++ b/Documents/DB_Tables_20141229.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="70">
   <si>
     <t xml:space="preserve">Table Name </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -283,6 +283,18 @@
   </si>
   <si>
     <t>구글 맵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VIEW_COUNT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIZE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -345,11 +357,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -660,29 +672,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2"/>
+      <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B3" t="s">
@@ -747,7 +759,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B11" t="s">
@@ -801,23 +813,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
+    <row r="16" spans="1:4">
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -830,392 +836,411 @@
       </c>
     </row>
     <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="3" t="s">
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>16</v>
       </c>
-      <c r="C22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>25</v>
       </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>17</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="B29" t="s">
         <v>20</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="3" t="s">
+    <row r="31" spans="1:4">
+      <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>35</v>
       </c>
-      <c r="C29" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>16</v>
       </c>
-      <c r="C30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="B31" t="s">
+    <row r="33" spans="1:4">
+      <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="B32" t="s">
+    <row r="34" spans="1:4">
+      <c r="B34" t="s">
         <v>34</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="3" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>16</v>
       </c>
-      <c r="C34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
         <v>43</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>17</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="B36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="B37" t="s">
-        <v>18</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
-      <c r="D37" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="38" spans="1:4">
       <c r="B38" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
         <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="B39" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="B40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="B41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="B42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="B43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="B44" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="B46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="B47" t="s">
         <v>20</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="3" t="s">
+    <row r="49" spans="1:4">
+      <c r="A49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
         <v>35</v>
       </c>
-      <c r="C47" t="s">
-        <v>26</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>16</v>
       </c>
-      <c r="C48" t="s">
-        <v>26</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="B49" t="s">
+    <row r="51" spans="1:4">
+      <c r="B51" t="s">
         <v>36</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C51" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="B50" t="s">
+    <row r="52" spans="1:4">
+      <c r="B52" t="s">
         <v>34</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="3" t="s">
+    <row r="54" spans="1:4">
+      <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>16</v>
       </c>
-      <c r="C52" t="s">
-        <v>26</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" t="s">
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
         <v>60</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
         <v>17</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C55" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="B54" t="s">
-        <v>18</v>
-      </c>
-      <c r="C54" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="B55" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="B56" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="C56" t="s">
-        <v>58</v>
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="B57" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C57" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="B58" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="B59" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="B60" t="s">
         <v>20</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="3" t="s">
+    <row r="62" spans="1:4">
+      <c r="A62" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B62" t="s">
         <v>36</v>
-      </c>
-      <c r="C60" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="B62" t="s">
-        <v>64</v>
       </c>
       <c r="C62" t="s">
         <v>37</v>
       </c>
-      <c r="D62" t="s">
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="B64" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64" t="s">
+        <v>37</v>
+      </c>
+      <c r="D64" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="B63" t="s">
+    <row r="65" spans="2:3">
+      <c r="B65" t="s">
         <v>19</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C65" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>